<commit_message>
updating requirements to more fully match what is wanted.
</commit_message>
<xml_diff>
--- a/Documents/report.xlsx
+++ b/Documents/report.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="log" localSheetId="1">Time!$A$1:$C$62</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,8 +27,22 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="log" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr prompt="0" codePage="437" sourceFile="C:\cygwin64\home\Michael\dev\ParallelRayTracer\log.csv" tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="32">
   <si>
     <t>Michael Warren</t>
   </si>
@@ -519,6 +536,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log" growShrinkType="overwriteClear" fillFormulas="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,7 +808,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +850,7 @@
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
       <c r="M2" s="1">
-        <v>41713</v>
+        <v>41718</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -918,7 +939,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="6">
         <f>SUMIF(Time!A:A,A5,Time!D:D)</f>
-        <v>13.417777777777777</v>
+        <v>16.593333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -946,7 +967,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="6">
         <f>SUMIF(Time!A:A,A6,Time!D:D)</f>
-        <v>1.6902777777777775</v>
+        <v>2.9663888888888885</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1111,7 +1132,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="6">
         <f>SUM(K4:K11)</f>
-        <v>29.273055555555555</v>
+        <v>33.724722222222219</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1219,7 +1240,7 @@
       </c>
       <c r="B20" s="13">
         <f>SUMIFS(Time!D:D,Time!B:B,"&gt;="&amp;M2)</f>
-        <v>12.22777777777778</v>
+        <v>4.4516666666666671</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1415,11 +1436,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1454,7 +1473,7 @@
         <v>41704.125</v>
       </c>
       <c r="D2" s="16">
-        <f t="shared" ref="D2:D56" si="0">IFERROR(MINUTE(C2-B2)/60+HOUR(C2-B2)+SECOND(C2-B2)/3600,0)</f>
+        <f t="shared" ref="D2:D62" si="0">IFERROR(MINUTE(C2-B2)/60+HOUR(C2-B2)+SECOND(C2-B2)/3600,0)</f>
         <v>3</v>
       </c>
     </row>
@@ -2266,6 +2285,94 @@
       <c r="D56" s="16">
         <f t="shared" si="0"/>
         <v>3.0555555555555557E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1">
+        <v>41718.823206018518</v>
+      </c>
+      <c r="C57" s="1">
+        <v>41718.846122685187</v>
+      </c>
+      <c r="D57" s="16">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="1">
+        <v>41718.846319444441</v>
+      </c>
+      <c r="C58" s="1">
+        <v>41718.897256944445</v>
+      </c>
+      <c r="D58" s="16">
+        <f t="shared" si="0"/>
+        <v>1.2225000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="1">
+        <v>41720.644143518519</v>
+      </c>
+      <c r="C59" s="1">
+        <v>41720.646377314813</v>
+      </c>
+      <c r="D59" s="16">
+        <f t="shared" si="0"/>
+        <v>5.3611111111111116E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1">
+        <v>41720.646458333336</v>
+      </c>
+      <c r="C60" s="1">
+        <v>41720.71539351852</v>
+      </c>
+      <c r="D60" s="16">
+        <f t="shared" si="0"/>
+        <v>1.6544444444444444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1">
+        <v>41720.72351851852</v>
+      </c>
+      <c r="C61" s="1">
+        <v>41720.763981481483</v>
+      </c>
+      <c r="D61" s="16">
+        <f t="shared" si="0"/>
+        <v>0.97111111111111115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1">
+        <v>41720.764502314814</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating report and design
</commit_message>
<xml_diff>
--- a/Documents/report.xlsx
+++ b/Documents/report.xlsx
@@ -9,15 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="log_2" localSheetId="1">Time!$A$1:$C$94</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,22 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="log" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\cygwin64\home\Michael\dev\ParallelRayTracer\log.csv" tab="0" comma="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="32">
   <si>
     <t>Michael Warren</t>
   </si>
@@ -96,9 +79,6 @@
     <t>Design</t>
   </si>
   <si>
-    <t>Math Unit Test  and code</t>
-  </si>
-  <si>
     <t>Sequential Ray Tracer Tests and code</t>
   </si>
   <si>
@@ -124,24 +104,27 @@
   </si>
   <si>
     <t xml:space="preserve">Changes in Scope, Schedule, and Cost: </t>
+  </si>
+  <si>
+    <t>On schedule for hours</t>
+  </si>
+  <si>
+    <t>Math Unit Test and code</t>
   </si>
   <si>
     <t xml:space="preserve">Scripture
 " 15 For behold, we are in bondage to the [senior project] and are taxed with a tax which is grievous to be borne..." - Mosiah 7:15
-"The sleep of a labouring man is sweet, whether he eat little or much: but the abundance of the rich will not suffer him to sleep. " Ecclesiastes 5:12
+"Even the youths shall faint and be weary, and the young men shall utterly fall: " Isaiah 40:30
 </t>
   </si>
   <si>
-    <t>Accomplishments: Lots of reasearch done already. Requierments are done. Design is started.</t>
-  </si>
-  <si>
-    <t>Problems: Baby not letting me or my wife sleep as much as we want. Going out of town this weekend. Some more research may be required.</t>
-  </si>
-  <si>
-    <t>On schedule for hours</t>
-  </si>
-  <si>
-    <t>Will try to catch up on some time lost this week so I can be ahead of hours again. (scheduleStatus = min(scheduleHoursStatus, scheduleDateStatus))</t>
+    <t>Problems: Baby not letting me or my wife sleep as much as we want. When out of town this weekend. Some more research may be required. Due to finding great math library may not spend lots of time on math unit tests. Hopefully other areas will absorb more time.</t>
+  </si>
+  <si>
+    <t>Accomplishments: First of many unit tests have been written, good start on Sequential Ray tracer, found great math library that should do most everything I need done. Managed not to get behind on hours. Design mostly finished.</t>
+  </si>
+  <si>
+    <t>Will try to catch up on some time lost this week so I can be ahead of hours again.</t>
   </si>
 </sst>
 </file>
@@ -540,10 +523,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log_2" growShrinkType="overwriteClear" fillFormulas="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -809,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,8 +919,8 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="6">
-        <f ca="1">SUMIF(Time!A:A,A5,Time!D:D)</f>
-        <v>22.042777777777783</v>
+        <f>SUMIF(Time!A:A,A5,Time!D:D)</f>
+        <v>22.930277777777786</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -999,12 +978,12 @@
       <c r="J7" s="5"/>
       <c r="K7" s="6">
         <f>SUMIF(Time!A:A,A7,Time!D:D)</f>
-        <v>7.9541666666666675</v>
+        <v>8.2722222222222239</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1013,7 +992,9 @@
         <v>41740</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>41730</v>
+      </c>
       <c r="F8" s="4">
         <v>41753</v>
       </c>
@@ -1025,12 +1006,12 @@
       <c r="J8" s="5"/>
       <c r="K8" s="6">
         <f>SUMIF(Time!A:A,A8,Time!D:D)</f>
-        <v>0</v>
+        <v>0.11833333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1039,7 +1020,9 @@
         <v>41753</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>41730</v>
+      </c>
       <c r="F9" s="4">
         <v>41764</v>
       </c>
@@ -1051,12 +1034,12 @@
       <c r="J9" s="5"/>
       <c r="K9" s="6">
         <f>SUMIF(Time!A:A,A9,Time!D:D)</f>
-        <v>0</v>
+        <v>2.3405555555555555</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -1082,7 +1065,7 @@
     </row>
     <row r="11" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -1108,28 +1091,28 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="5">
         <f>SUM(I4:I11)</f>
@@ -1137,13 +1120,13 @@
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="6">
-        <f ca="1">SUM(K4:K11)</f>
-        <v>47.959166666666668</v>
+        <f>SUM(K4:K11)</f>
+        <v>51.623611111111117</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -1199,7 +1182,7 @@
     </row>
     <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1227,7 +1210,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1242,11 +1225,11 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="13">
-        <f ca="1">SUMIFS(Time!D:D,Time!B:B,"&gt;="&amp;M2)</f>
-        <v>8.1722222222222225</v>
+        <f>SUMIFS(Time!D:D,Time!B:B,"&gt;="&amp;M2)</f>
+        <v>11.836666666666668</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1260,7 +1243,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="14">
         <v>156</v>
@@ -1277,7 +1260,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1320,7 +1303,7 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -1445,15 +1428,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2444,7 +2427,7 @@
         <v>41722.834305555552</v>
       </c>
       <c r="D66" s="16">
-        <f t="shared" ref="D66:D94" si="1">IFERROR(MINUTE(C66-B66)/60+HOUR(C66-B66)+SECOND(C66-B66)/3600,0)</f>
+        <f t="shared" ref="D66:D106" si="1">IFERROR(MINUTE(C66-B66)/60+HOUR(C66-B66)+SECOND(C66-B66)/3600,0)</f>
         <v>1.0833333333333334E-2</v>
       </c>
     </row>
@@ -2861,12 +2844,191 @@
         <v>41730.875092592592</v>
       </c>
       <c r="C94" s="17">
-        <f ca="1">NOW()</f>
-        <v>41730.896799074071</v>
+        <v>41730.887291666666</v>
       </c>
       <c r="D94" s="16">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.52083333333333337</v>
+        <f t="shared" si="1"/>
+        <v>0.29277777777777775</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>27</v>
+      </c>
+      <c r="B95" s="17">
+        <v>41730.887291666666</v>
+      </c>
+      <c r="C95" s="17">
+        <v>41730.892222222225</v>
+      </c>
+      <c r="D95" s="16">
+        <f t="shared" si="1"/>
+        <v>0.11833333333333333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96" s="17">
+        <v>41730.892222222225</v>
+      </c>
+      <c r="C96" s="17">
+        <v>41730.908935185187</v>
+      </c>
+      <c r="D96" s="16">
+        <f t="shared" si="1"/>
+        <v>0.40111111111111114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97" s="17">
+        <v>41731.749699074076</v>
+      </c>
+      <c r="C97" s="17">
+        <v>41731.751331018517</v>
+      </c>
+      <c r="D97" s="16">
+        <f t="shared" si="1"/>
+        <v>3.9166666666666669E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="17">
+        <v>41731.751331018517</v>
+      </c>
+      <c r="C98" s="17">
+        <v>41731.755520833336</v>
+      </c>
+      <c r="D98" s="16">
+        <f t="shared" si="1"/>
+        <v>0.10055555555555556</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" s="17">
+        <v>41731.755532407406</v>
+      </c>
+      <c r="C99" s="17">
+        <v>41731.778969907406</v>
+      </c>
+      <c r="D99" s="16">
+        <f t="shared" si="1"/>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="17">
+        <v>41731.778969907406</v>
+      </c>
+      <c r="C100" s="17">
+        <v>41731.804942129631</v>
+      </c>
+      <c r="D100" s="16">
+        <f t="shared" si="1"/>
+        <v>0.62333333333333341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" s="17">
+        <v>41731.804942129631</v>
+      </c>
+      <c r="C101" s="17">
+        <v>41731.811168981483</v>
+      </c>
+      <c r="D101" s="16">
+        <f t="shared" si="1"/>
+        <v>0.14944444444444444</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102" s="17">
+        <v>41731.811168981483</v>
+      </c>
+      <c r="C102" s="17">
+        <v>41731.828935185185</v>
+      </c>
+      <c r="D102" s="16">
+        <f t="shared" si="1"/>
+        <v>0.42638888888888893</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="17">
+        <v>41731.832708333335</v>
+      </c>
+      <c r="C103" s="17">
+        <v>41731.847071759257</v>
+      </c>
+      <c r="D103" s="16">
+        <f t="shared" si="1"/>
+        <v>0.34472222222222221</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="17">
+        <v>41731.867361111108</v>
+      </c>
+      <c r="C104" s="17">
+        <v>41731.892604166664</v>
+      </c>
+      <c r="D104" s="16">
+        <f t="shared" si="1"/>
+        <v>0.60583333333333333</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" s="17">
+        <v>41731.892604166664</v>
+      </c>
+      <c r="C105" s="17">
+        <v>41731.897997685184</v>
+      </c>
+      <c r="D105" s="16">
+        <f t="shared" si="1"/>
+        <v>0.12944444444444445</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="17">
+        <v>41731.898009259261</v>
+      </c>
+      <c r="C106" s="17">
+        <v>41731.9143287037</v>
+      </c>
+      <c r="D106" s="16">
+        <f t="shared" si="1"/>
+        <v>0.39166666666666672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>